<commit_message>
pushing this weeks non pos stuff
</commit_message>
<xml_diff>
--- a/PREM/Zeitaufzeichnungen/ZeitaufzeichnungSeptember.xlsx
+++ b/PREM/Zeitaufzeichnungen/ZeitaufzeichnungSeptember.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Documents\GitHub\3DHIF\PREM\Zeitaufzeichnungen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github_for_school\3DHIF_D_2025_26\PREM\Zeitaufzeichnungen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B05D905-7D14-45E2-A74C-D42A24AF3B25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3137FCD3-ED70-4929-AC14-AE8D88093E13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="1755" windowWidth="26340" windowHeight="11835" xr2:uid="{1D8CD667-A7EF-4BFB-8417-310C3CB05619}"/>
+    <workbookView xWindow="225" yWindow="1950" windowWidth="26340" windowHeight="11835" xr2:uid="{1D8CD667-A7EF-4BFB-8417-310C3CB05619}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -423,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92603408-C500-4ED2-8432-1BCBCFD84CD1}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,6 +496,25 @@
         <v>45</v>
       </c>
     </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>45922</v>
+      </c>
+      <c r="D7">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>45926</v>
+      </c>
+      <c r="B8">
+        <v>45</v>
+      </c>
+      <c r="D8">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:D1"/>

</xml_diff>